<commit_message>
Rev 2 IO module complete
</commit_message>
<xml_diff>
--- a/Hardware/Boards/Layout Studies /fpga module layout study.xlsx
+++ b/Hardware/Boards/Layout Studies /fpga module layout study.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/Desktop/Projects/DICE/Hardware/Boards/Layout Studies /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CD5F77-4926-A947-9BF0-ACFE910DD2A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D043425B-5464-AD46-AF2E-D99A411C3A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20280" xr2:uid="{4216863B-A6B5-8642-A477-1124D4538903}"/>
+    <workbookView xWindow="0" yWindow="2060" windowWidth="34560" windowHeight="20280" xr2:uid="{4216863B-A6B5-8642-A477-1124D4538903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,15 +439,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>513080</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>5080</xdr:colOff>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>771313</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -463,8 +463,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2981960" y="8585200"/>
-          <a:ext cx="3228340" cy="1714500"/>
+          <a:off x="6642947" y="1676400"/>
+          <a:ext cx="3255433" cy="1714500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -507,16 +507,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>736600</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>673100</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>469901</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -531,8 +531,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6515100" y="1752600"/>
-          <a:ext cx="3238500" cy="1714500"/>
+          <a:off x="3022600" y="8610600"/>
+          <a:ext cx="3255434" cy="1714500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -757,9 +757,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:colOff>73025</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>136525</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -775,7 +775,7 @@
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
           <a:off x="3168650" y="6445250"/>
-          <a:ext cx="1212850" cy="349250"/>
+          <a:ext cx="1031875" cy="193675"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1406,8 +1406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1F5B37-6EE7-DB40-AE34-5E8BB1922385}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" workbookViewId="0">
-      <selection activeCell="P61" sqref="P61"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="75" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>